<commit_message>
Added comments to Structure Comparison Table
</commit_message>
<xml_diff>
--- a/dgl/visualization/results_structureFinding/structureComparisonTable.xlsx
+++ b/dgl/visualization/results_structureFinding/structureComparisonTable.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Documents\Datoteke_za_solo\MAG\magistrska\dgl\visualization\results_structureFinding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bsmrdelj.CT\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DDC6DC-FF93-4002-91EF-B53DABE02E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="1980" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28590" windowHeight="6375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +18,163 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Benjamin Smrdelj</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Benjamin Smrdelj:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hydrolysis (addition of water)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Benjamin Smrdelj:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rearrangement of atoms within a molecule</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Benjamin Smrdelj:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Joining of two molecules (using energy usually derived from the breakdown of ATP)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Benjamin Smrdelj:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Removal of groups of atoms without hydrolysis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Benjamin Smrdelj:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Oxidation-reduction in which oxygen and hydrogen are gained or lost.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Benjamin Smrdelj:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Transfer of functional groups, such as an amino group, acetyl group, or phosphate group</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Hydrolase</t>
   </si>
@@ -154,14 +308,17 @@
     <t>Najpogostejša skupina pri transferazah.</t>
   </si>
   <si>
-    <t>Najpogostejša skupina pri ligazah.</t>
+    <t>Pomembna skupina pri izomerazah.</t>
+  </si>
+  <si>
+    <t>Najpogostejša skupina pri ligazah (del ATP-ja).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +333,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,7 +417,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -19508,9 +19678,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pisarna">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -19548,7 +19718,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pisarna">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -19583,23 +19753,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -19635,26 +19788,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pisarna">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -19827,12 +19963,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19875,7 +20011,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -19888,7 +20024,9 @@
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -20134,5 +20272,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>